<commit_message>
Update mining training set
</commit_message>
<xml_diff>
--- a/data/aa_cleaned_up_serina_min_grp_size_50.xlsx
+++ b/data/aa_cleaned_up_serina_min_grp_size_50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/Wageningen_UR/github/mibig_training_set_build_test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824918E2-EC87-414B-95E1-3ADDA00B784C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CA949-E4A0-7244-82C8-F5FD4C8A2908}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="460" windowWidth="17540" windowHeight="14440" xr2:uid="{4842E814-1572-C544-BEDF-D92B2EFA245C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>Cysteine</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>Bulky mainly phenyl derivatives</t>
+  </si>
+  <si>
+    <t>lea</t>
   </si>
 </sst>
 </file>
@@ -778,7 +781,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H37"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,6 +1087,9 @@
       <c r="F14" t="s">
         <v>91</v>
       </c>
+      <c r="H14" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Update machine learning scripts
</commit_message>
<xml_diff>
--- a/data/aa_cleaned_up_serina_min_grp_size_50.xlsx
+++ b/data/aa_cleaned_up_serina_min_grp_size_50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/Wageningen_UR/github/mibig_training_set_build_test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CA949-E4A0-7244-82C8-F5FD4C8A2908}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE114E-D1B9-C64E-A25E-20F9FAAB5D2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="460" windowWidth="17540" windowHeight="14440" xr2:uid="{4842E814-1572-C544-BEDF-D92B2EFA245C}"/>
+    <workbookView xWindow="8060" yWindow="920" windowWidth="17540" windowHeight="14440" xr2:uid="{4842E814-1572-C544-BEDF-D92B2EFA245C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,9 +381,6 @@
     <t>kyn</t>
   </si>
   <si>
-    <t>Small hydrophilic</t>
-  </si>
-  <si>
     <t>REJECT</t>
   </si>
   <si>
@@ -418,6 +415,9 @@
   </si>
   <si>
     <t>lea</t>
+  </si>
+  <si>
+    <t>Small non-hydrophobic</t>
   </si>
 </sst>
 </file>
@@ -441,12 +441,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -461,9 +467,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A484F7-A651-C849-88AA-42C366A24300}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,28 +802,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -855,7 +862,7 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
@@ -865,7 +872,7 @@
         <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -888,7 +895,7 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -905,7 +912,7 @@
         <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5" t="s">
         <v>101</v>
@@ -1048,7 +1055,7 @@
         <v>82</v>
       </c>
       <c r="H12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1088,7 +1095,7 @@
         <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1147,7 +1154,7 @@
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1222,7 +1229,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>